<commit_message>
adding study title and description
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>contact_first_name</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>contact_institution</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
   <si>
     <t>workflow</t>
@@ -583,7 +589,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -593,11 +599,13 @@
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,6 +623,12 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -645,37 +659,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -696,7 +710,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -749,103 +763,103 @@
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -868,13 +882,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -895,7 +909,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -923,28 +937,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -968,16 +982,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1001,16 +1015,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding in ability to filter by core and full dwc terms
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="294">
   <si>
     <t>First Name</t>
   </si>
@@ -87,6 +87,9 @@
     <t>environmental_medium</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
     <t>modified</t>
   </si>
   <si>
@@ -117,6 +120,9 @@
     <t>institutionCode</t>
   </si>
   <si>
+    <t>collectionCode</t>
+  </si>
+  <si>
     <t>datasetName</t>
   </si>
   <si>
@@ -141,6 +147,9 @@
     <t>occurrenceID</t>
   </si>
   <si>
+    <t>catalogNumber</t>
+  </si>
+  <si>
     <t>recordNumber</t>
   </si>
   <si>
@@ -342,6 +351,9 @@
     <t>island</t>
   </si>
   <si>
+    <t>country</t>
+  </si>
+  <si>
     <t>countryCode</t>
   </si>
   <si>
@@ -402,6 +414,12 @@
     <t>geodeticDatum</t>
   </si>
   <si>
+    <t>coordinateUncertaintyInMeters</t>
+  </si>
+  <si>
+    <t>coordinatePrecision</t>
+  </si>
+  <si>
     <t>pointRadiusSpatialFit</t>
   </si>
   <si>
@@ -589,6 +607,9 @@
   </si>
   <si>
     <t>phylum</t>
+  </si>
+  <si>
+    <t>class</t>
   </si>
   <si>
     <t>order</t>
@@ -1293,7 +1314,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:JS1"/>
+  <dimension ref="A1:JZ1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1311,272 +1332,279 @@
     <col min="10" max="10" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="22" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="11" bestFit="1" customWidth="1"/>
-    <col min="57" max="58" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="15" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="6" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="14" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="10" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="7" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="12" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="23" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="19" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="13" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="15" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="6" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="14" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="10" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="7" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="12" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="23" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="19" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="13" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="133" max="133" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="25" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="13" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="21" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="12" bestFit="1" customWidth="1"/>
-    <col min="158" max="159" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="23" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="14" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="21" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="22" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="26" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="9" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="12" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="22" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="237" max="238" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="13" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="244" max="244" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="245" max="245" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="254" max="254" width="19" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="14" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="4" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="25" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="13" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="21" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="12" bestFit="1" customWidth="1"/>
+    <col min="164" max="165" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="23" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="14" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="209" max="209" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="210" max="210" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="21" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="225" max="225" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="22" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="26" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="9" bestFit="1" customWidth="1"/>
+    <col min="231" max="231" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="232" max="232" width="12" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="235" max="235" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="240" max="240" width="22" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="244" max="245" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="13" bestFit="1" customWidth="1"/>
+    <col min="249" max="249" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="250" max="250" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="254" max="254" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="19" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="14" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="273" max="273" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="275" max="275" width="4" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="279" max="279" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="281" max="281" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="282" max="282" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="283" max="283" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="284" max="284" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="285" max="285" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="286" max="286" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:279">
+    <row r="1" spans="1:286">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1629,10 +1657,10 @@
         <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>27</v>
@@ -2244,175 +2272,196 @@
         <v>229</v>
       </c>
       <c r="HO1" s="1" t="s">
-        <v>22</v>
+        <v>230</v>
       </c>
       <c r="HP1" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="HQ1" s="1" t="s">
-        <v>164</v>
+        <v>232</v>
       </c>
       <c r="HR1" s="1" t="s">
-        <v>40</v>
+        <v>233</v>
       </c>
       <c r="HS1" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="HT1" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="HU1" s="1" t="s">
-        <v>135</v>
+        <v>236</v>
       </c>
       <c r="HV1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="HW1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="HX1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="HY1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="HZ1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="IA1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="IB1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="IC1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="ID1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="IE1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="IF1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="IG1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="IH1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="II1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="IJ1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="IK1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="IL1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="IM1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="IN1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="IO1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="IP1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="IQ1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="IR1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="IS1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="IT1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="IU1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="IV1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="IW1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="IX1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="IY1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="IZ1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="HW1" s="1" t="s">
+      <c r="JA1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="JB1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="JC1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="JD1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="JE1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="JF1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="JG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="JH1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="JI1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="JJ1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="JK1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="JL1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="JM1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="JN1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="JO1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="HX1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="HY1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="HZ1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="IA1" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="IB1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="IC1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="ID1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="IE1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="IF1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="IG1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="IH1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="II1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="IJ1" s="1" t="s">
+      <c r="JP1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="JQ1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="JR1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="IK1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="IL1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="IM1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="IN1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="IO1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="IP1" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="IQ1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="IR1" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="IS1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="IT1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="IU1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="IV1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="IW1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="IX1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="IY1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="IZ1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="JA1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="JB1" s="1" t="s">
+      <c r="JS1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="JT1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="JC1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="JD1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="JE1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="JF1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="JG1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="JH1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="JI1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="JJ1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="JK1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="JL1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="JM1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="JN1" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="JO1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="JP1" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="JQ1" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="JR1" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="JS1" s="1" t="s">
-        <v>242</v>
+      <c r="JU1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="JV1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="JW1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="JX1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="JY1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="JZ1" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2433,7 +2482,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2479,82 +2528,82 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2577,16 +2626,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -2607,7 +2656,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2635,28 +2684,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2680,16 +2729,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -2713,16 +2762,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>